<commit_message>
Added corrected version of inclusion_sets
As of 17-09, excluding MTT13 LAB52 and MTT42 LAB18 from primary analysis
</commit_message>
<xml_diff>
--- a/other-data/inclusion_sets.xlsx
+++ b/other-data/inclusion_sets.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gapsm\OneDrive\Outros\OneNote\bri-analysis\other-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/Brazilian Reproducibility Initiative/Análise/bri-analysis-fixing-data-issues(olavo)/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFBC925-D64A-4942-9E06-6A3D97F25696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35896825-338D-9E4F-BBAB-F4E5411A92BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="27620" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2217" uniqueCount="214">
   <si>
     <t>EXP</t>
   </si>
@@ -656,13 +656,19 @@
   </si>
   <si>
     <t>Lack of technical replicates</t>
+  </si>
+  <si>
+    <t>Checking of suspect data with labs led to changes of group labels and submission of new data, reducing confidence on whether all results had been accurately and fully reported.</t>
+  </si>
+  <si>
+    <t>Because of an error in the protocol, experiment used 20 uM instead of 20 mM NaSal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +684,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -687,7 +699,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -695,14 +707,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,13 +1040,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="G144" sqref="G144"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="AA89" sqref="AA89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="20" max="20" width="12.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1239,7 +1272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1346,7 +1379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1453,7 +1486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1545,7 +1578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1637,7 +1670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1732,7 +1765,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1827,7 +1860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1853,7 +1886,7 @@
         <v>0.29299999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1945,7 +1978,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -2031,7 +2064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -2048,7 +2081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2065,7 +2098,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -2082,7 +2115,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -2099,7 +2132,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -2116,7 +2149,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2217,7 +2250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -2243,7 +2276,7 @@
         <v>0.311</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -2344,7 +2377,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -2451,7 +2484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -2558,7 +2591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2665,7 +2698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -2766,7 +2799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -2792,7 +2825,7 @@
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2893,7 +2926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -2997,7 +3030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -3101,7 +3134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -3205,7 +3238,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -3306,7 +3339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -3332,7 +3365,7 @@
         <v>0.51800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -3433,7 +3466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -3534,7 +3567,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -3638,7 +3671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -3739,7 +3772,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -3840,7 +3873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -3935,7 +3968,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -4036,7 +4069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -4140,7 +4173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -4232,7 +4265,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -4336,7 +4369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -4437,7 +4470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -4529,7 +4562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -4630,7 +4663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -4647,7 +4680,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -4664,7 +4697,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -4681,7 +4714,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -4698,7 +4731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -4781,7 +4814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -4798,7 +4831,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -4815,7 +4848,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -4832,7 +4865,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -4849,7 +4882,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>92</v>
       </c>
@@ -4866,7 +4899,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>92</v>
       </c>
@@ -4883,7 +4916,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -4966,7 +4999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -5058,7 +5091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -5150,7 +5183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -5242,7 +5275,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>95</v>
       </c>
@@ -5343,7 +5376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -5444,7 +5477,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>95</v>
       </c>
@@ -5539,7 +5572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -5555,12 +5588,6 @@
       <c r="E62" t="s">
         <v>41</v>
       </c>
-      <c r="F62" t="s">
-        <v>41</v>
-      </c>
-      <c r="G62" t="s">
-        <v>41</v>
-      </c>
       <c r="H62" t="s">
         <v>41</v>
       </c>
@@ -5583,10 +5610,16 @@
         <v>1.3</v>
       </c>
       <c r="S62" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="T62" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="U62" t="s">
+        <v>61</v>
+      </c>
+      <c r="V62" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="W62">
         <v>0.13700000000000001</v>
@@ -5637,7 +5670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>97</v>
       </c>
@@ -5656,9 +5689,6 @@
       <c r="F63" t="s">
         <v>41</v>
       </c>
-      <c r="G63" t="s">
-        <v>41</v>
-      </c>
       <c r="H63" t="s">
         <v>41</v>
       </c>
@@ -5735,7 +5765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>97</v>
       </c>
@@ -5754,9 +5784,6 @@
       <c r="F64" t="s">
         <v>41</v>
       </c>
-      <c r="G64" t="s">
-        <v>41</v>
-      </c>
       <c r="H64" t="s">
         <v>41</v>
       </c>
@@ -5830,7 +5857,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -5931,7 +5958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -6026,7 +6053,7 @@
         <v>778.66666666666697</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -6124,7 +6151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>107</v>
       </c>
@@ -6141,7 +6168,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>107</v>
       </c>
@@ -6224,7 +6251,7 @@
         <v>375.33333333333297</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>107</v>
       </c>
@@ -6304,7 +6331,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>107</v>
       </c>
@@ -6390,7 +6417,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>115</v>
       </c>
@@ -6488,7 +6515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>115</v>
       </c>
@@ -6586,7 +6613,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>115</v>
       </c>
@@ -6612,7 +6639,7 @@
         <v>0.29799999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>118</v>
       </c>
@@ -6710,7 +6737,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>118</v>
       </c>
@@ -6736,7 +6763,7 @@
         <v>0.316</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>118</v>
       </c>
@@ -6834,7 +6861,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>121</v>
       </c>
@@ -6929,7 +6956,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -7027,7 +7054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>121</v>
       </c>
@@ -7053,7 +7080,7 @@
         <v>0.23300000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>123</v>
       </c>
@@ -7157,7 +7184,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>123</v>
       </c>
@@ -7264,7 +7291,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>123</v>
       </c>
@@ -7371,7 +7398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>125</v>
       </c>
@@ -7397,7 +7424,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>125</v>
       </c>
@@ -7492,7 +7519,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>125</v>
       </c>
@@ -7584,7 +7611,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>128</v>
       </c>
@@ -7603,9 +7630,6 @@
       <c r="F87" t="s">
         <v>41</v>
       </c>
-      <c r="G87" t="s">
-        <v>41</v>
-      </c>
       <c r="H87" t="s">
         <v>41</v>
       </c>
@@ -7691,7 +7715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>128</v>
       </c>
@@ -7710,9 +7734,6 @@
       <c r="F88" t="s">
         <v>41</v>
       </c>
-      <c r="G88" t="s">
-        <v>41</v>
-      </c>
       <c r="H88" t="s">
         <v>41</v>
       </c>
@@ -7798,7 +7819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>128</v>
       </c>
@@ -7814,24 +7835,6 @@
       <c r="E89" t="s">
         <v>41</v>
       </c>
-      <c r="F89" t="s">
-        <v>41</v>
-      </c>
-      <c r="G89" t="s">
-        <v>41</v>
-      </c>
-      <c r="H89" t="s">
-        <v>41</v>
-      </c>
-      <c r="I89" t="s">
-        <v>41</v>
-      </c>
-      <c r="J89" t="s">
-        <v>41</v>
-      </c>
-      <c r="K89" t="s">
-        <v>41</v>
-      </c>
       <c r="L89" t="s">
         <v>42</v>
       </c>
@@ -7851,10 +7854,16 @@
         <v>1.6</v>
       </c>
       <c r="S89" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="T89" t="s">
         <v>43</v>
+      </c>
+      <c r="U89" t="s">
+        <v>50</v>
+      </c>
+      <c r="V89" t="s">
+        <v>213</v>
       </c>
       <c r="W89">
         <v>1</v>
@@ -7902,7 +7911,7 @@
         <v>778.66666666666697</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>131</v>
       </c>
@@ -8003,7 +8012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -8104,7 +8113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>131</v>
       </c>
@@ -8130,7 +8139,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -8156,7 +8165,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>133</v>
       </c>
@@ -8257,7 +8266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>133</v>
       </c>
@@ -8358,7 +8367,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>135</v>
       </c>
@@ -8450,7 +8459,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>135</v>
       </c>
@@ -8539,7 +8548,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>135</v>
       </c>
@@ -8628,7 +8637,7 @@
         <v>215.5</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>140</v>
       </c>
@@ -8720,7 +8729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>140</v>
       </c>
@@ -8746,7 +8755,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>140</v>
       </c>
@@ -8835,7 +8844,7 @@
         <v>215.5</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>142</v>
       </c>
@@ -8939,7 +8948,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>142</v>
       </c>
@@ -9037,7 +9046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>142</v>
       </c>
@@ -9063,7 +9072,7 @@
         <v>0.443</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>145</v>
       </c>
@@ -9167,7 +9176,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>145</v>
       </c>
@@ -9274,7 +9283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>145</v>
       </c>
@@ -9378,7 +9387,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>146</v>
       </c>
@@ -9470,7 +9479,7 @@
         <v>375.33333333333297</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>146</v>
       </c>
@@ -9559,7 +9568,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>146</v>
       </c>
@@ -9654,7 +9663,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>146</v>
       </c>
@@ -9749,7 +9758,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>147</v>
       </c>
@@ -9847,7 +9856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>147</v>
       </c>
@@ -9942,7 +9951,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>147</v>
       </c>
@@ -10040,7 +10049,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>150</v>
       </c>
@@ -10132,7 +10141,7 @@
         <v>588.75</v>
       </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>150</v>
       </c>
@@ -10227,7 +10236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>150</v>
       </c>
@@ -10322,7 +10331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>153</v>
       </c>
@@ -10423,7 +10432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>153</v>
       </c>
@@ -10524,7 +10533,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>153</v>
       </c>
@@ -10628,7 +10637,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>154</v>
       </c>
@@ -10711,7 +10720,7 @@
         <v>375.33333333333297</v>
       </c>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>154</v>
       </c>
@@ -10791,7 +10800,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>154</v>
       </c>
@@ -10877,7 +10886,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>154</v>
       </c>
@@ -10894,7 +10903,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>155</v>
       </c>
@@ -10989,7 +10998,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>155</v>
       </c>
@@ -11081,7 +11090,7 @@
         <v>375.33333333333297</v>
       </c>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>155</v>
       </c>
@@ -11179,7 +11188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>159</v>
       </c>
@@ -11277,7 +11286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>159</v>
       </c>
@@ -11369,7 +11378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>159</v>
       </c>
@@ -11467,7 +11476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>163</v>
       </c>
@@ -11571,7 +11580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>163</v>
       </c>
@@ -11675,7 +11684,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>163</v>
       </c>
@@ -11779,7 +11788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>167</v>
       </c>
@@ -11865,7 +11874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>167</v>
       </c>
@@ -11945,7 +11954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>167</v>
       </c>
@@ -12031,7 +12040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>167</v>
       </c>
@@ -12048,7 +12057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>170</v>
       </c>
@@ -12149,7 +12158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>170</v>
       </c>
@@ -12244,7 +12253,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>170</v>
       </c>
@@ -12333,7 +12342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>170</v>
       </c>
@@ -12425,7 +12434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>174</v>
       </c>
@@ -12526,7 +12535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>174</v>
       </c>
@@ -12539,9 +12548,6 @@
       <c r="D143" t="s">
         <v>41</v>
       </c>
-      <c r="E143" t="s">
-        <v>41</v>
-      </c>
       <c r="L143" t="s">
         <v>42</v>
       </c>
@@ -12621,7 +12627,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>174</v>
       </c>
@@ -12725,7 +12731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>179</v>
       </c>
@@ -12823,7 +12829,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>179</v>
       </c>
@@ -12912,7 +12918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>179</v>
       </c>
@@ -13004,7 +13010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>179</v>
       </c>
@@ -13105,7 +13111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>181</v>
       </c>
@@ -13206,7 +13212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>181</v>
       </c>
@@ -13307,7 +13313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>181</v>
       </c>
@@ -13396,7 +13402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>181</v>
       </c>
@@ -13488,7 +13494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>182</v>
       </c>
@@ -13514,7 +13520,7 @@
         <v>0.20100000000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>182</v>
       </c>
@@ -13609,7 +13615,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>182</v>
       </c>
@@ -13707,7 +13713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>183</v>
       </c>
@@ -13787,7 +13793,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>183</v>
       </c>
@@ -13873,7 +13879,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>183</v>
       </c>
@@ -13890,7 +13896,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>183</v>
       </c>
@@ -13970,7 +13976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>183</v>
       </c>
@@ -14053,7 +14059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>185</v>
       </c>
@@ -14151,7 +14157,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>185</v>
       </c>
@@ -14249,7 +14255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>185</v>
       </c>
@@ -14341,7 +14347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>189</v>
       </c>
@@ -14436,7 +14442,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>189</v>
       </c>
@@ -14528,7 +14534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>189</v>
       </c>
@@ -14554,7 +14560,7 @@
         <v>0.18099999999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>190</v>
       </c>
@@ -14646,7 +14652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>190</v>
       </c>
@@ -14741,7 +14747,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>190</v>
       </c>
@@ -14839,7 +14845,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>194</v>
       </c>
@@ -14934,7 +14940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>194</v>
       </c>
@@ -15029,7 +15035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>194</v>
       </c>
@@ -15124,7 +15130,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>194</v>
       </c>
@@ -15219,7 +15225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>197</v>
       </c>
@@ -15323,7 +15329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>197</v>
       </c>
@@ -15427,7 +15433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>197</v>
       </c>
@@ -15528,7 +15534,7 @@
         <v>375.33333333333297</v>
       </c>
     </row>
-    <row r="177" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>199</v>
       </c>
@@ -15608,7 +15614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>199</v>
       </c>
@@ -15694,7 +15700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>199</v>
       </c>
@@ -15780,7 +15786,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="180" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>199</v>
       </c>
@@ -15866,7 +15872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>204</v>
       </c>
@@ -15949,7 +15955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>204</v>
       </c>
@@ -16032,7 +16038,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="183" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>204</v>
       </c>
@@ -16118,7 +16124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>208</v>
       </c>
@@ -16207,7 +16213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>208</v>
       </c>
@@ -16302,7 +16308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>208</v>
       </c>
@@ -16397,7 +16403,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="187" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>208</v>
       </c>
@@ -16492,7 +16498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>209</v>
       </c>
@@ -16509,7 +16515,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="189" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>209</v>
       </c>
@@ -16526,7 +16532,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="190" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>209</v>
       </c>
@@ -16543,7 +16549,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="191" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>210</v>
       </c>
@@ -16638,7 +16644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>210</v>
       </c>
@@ -16730,7 +16736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>210</v>
       </c>

</xml_diff>

<commit_message>
Minor fix in validation decision reasons
</commit_message>
<xml_diff>
--- a/other-data/inclusion_sets.xlsx
+++ b/other-data/inclusion_sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/Brazilian Reproducibility Initiative/Análise/bri-analysis-fixing-data-issues(olavo)/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704CFAEE-4928-7248-9589-3F38B58254B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C16721-6CBE-5D40-9E9E-916CEF63F0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="26040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="221">
   <si>
     <t>EXP</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>analysis_only_80_power_a_posteriori_bigexp</t>
+  </si>
+  <si>
+    <t>Protocol deviation and insufficient sample size</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4511,7 +4514,7 @@
         <v>42</v>
       </c>
       <c r="W39" t="s">
-        <v>50</v>
+        <v>220</v>
       </c>
       <c r="X39" t="s">
         <v>53</v>
@@ -4832,7 +4835,7 @@
         <v>42</v>
       </c>
       <c r="W42" t="s">
-        <v>50</v>
+        <v>220</v>
       </c>
       <c r="X42" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Changed column name + revised data
Changed big_exp to bigexp in column name.
Changed MA ONLY to INCLUDE in analysis_all_exps
</commit_message>
<xml_diff>
--- a/other-data/inclusion_sets.xlsx
+++ b/other-data/inclusion_sets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/Brazilian Reproducibility Initiative/Análise/bri-analysis-fixing-data-issues(olavo)/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C16721-6CBE-5D40-9E9E-916CEF63F0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBE3F63-50F7-CC4E-B5E1-AAD303454ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="222">
   <si>
     <t>EXP</t>
   </si>
@@ -683,6 +683,9 @@
   </si>
   <si>
     <t>Protocol deviation and insufficient sample size</t>
+  </si>
+  <si>
+    <t>post hoc power bigexp</t>
   </si>
 </sst>
 </file>
@@ -1061,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="110" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1174,7 +1177,7 @@
         <v>24</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>25</v>
@@ -6836,7 +6839,7 @@
         <v>0.122</v>
       </c>
       <c r="E72" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="G72" t="s">
         <v>103</v>
@@ -10580,10 +10583,10 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="E114" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="F114" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="G114" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Fixed inconsistency in MTT18 LAB1 sets
</commit_message>
<xml_diff>
--- a/other-data/inclusion_sets.xlsx
+++ b/other-data/inclusion_sets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/Brazilian Reproducibility Initiative/Análise/bri-analysis-fixing-data-issues(olavo)/other-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/bri-analysis-pp-main/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A9591E-281A-8449-9833-0283408A1255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCC7A15-7516-F84B-92C3-1762C4ABB5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="221">
   <si>
     <t>EXP</t>
   </si>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6151,6 +6151,15 @@
       <c r="F65" t="s">
         <v>103</v>
       </c>
+      <c r="I65" t="s">
+        <v>103</v>
+      </c>
+      <c r="J65" t="s">
+        <v>103</v>
+      </c>
+      <c r="L65" t="s">
+        <v>103</v>
+      </c>
       <c r="M65" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Fixed inconsistency in MTT18 LAB1 (now fully)
</commit_message>
<xml_diff>
--- a/other-data/inclusion_sets.xlsx
+++ b/other-data/inclusion_sets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/bri-analysis-pp-main/other-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/bri-analysis-pp-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCC7A15-7516-F84B-92C3-1762C4ABB5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC8C075-9ED6-CB40-92B7-53C06B21DD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="221">
   <si>
     <t>EXP</t>
   </si>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" workbookViewId="0">
-      <selection activeCell="L65" sqref="L65"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6151,10 +6151,16 @@
       <c r="F65" t="s">
         <v>103</v>
       </c>
+      <c r="H65" t="s">
+        <v>103</v>
+      </c>
       <c r="I65" t="s">
         <v>103</v>
       </c>
       <c r="J65" t="s">
+        <v>103</v>
+      </c>
+      <c r="K65" t="s">
         <v>103</v>
       </c>
       <c r="L65" t="s">

</xml_diff>